<commit_message>
update BoltGrade to add the parameter k_rd req'd by AS4100 9.2.2.1
</commit_message>
<xml_diff>
--- a/src/utilityscripts/steel/data/steel_data.xlsx
+++ b/src/utilityscripts/steel/data/steel_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean Kane\PycharmProjects\utilityscripts\utilityscripts\steel\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sean.kane\programming\utilityscripts\src\utilityscripts\steel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD4AA5B-928F-46FD-8C45-7B51A51A759E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF815038-825E-45D7-8810-9D70A27C3F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{2C3896B0-8573-48C6-A232-BE22E9D89C30}"/>
+    <workbookView xWindow="-28920" yWindow="135" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{2C3896B0-8573-48C6-A232-BE22E9D89C30}"/>
   </bookViews>
   <sheets>
     <sheet name="is" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3260" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3261" uniqueCount="532">
   <si>
     <t>d</t>
   </si>
@@ -1644,6 +1644,9 @@
   </si>
   <si>
     <t>d_f</t>
+  </si>
+  <si>
+    <t>k_rd</t>
   </si>
 </sst>
 </file>
@@ -1662,11 +1665,11 @@
     <numFmt numFmtId="172" formatCode="0.000"/>
     <numFmt numFmtId="173" formatCode="0&quot; kg / m&quot;"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tinos"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1684,14 +1687,14 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="Tinos"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tinos"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1706,6 +1709,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1728,7 +1737,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -1831,15 +1840,33 @@
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="167">
+  <dxfs count="168">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Roboto"/>
+        <scheme val="major"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -4021,7 +4048,7 @@
         <vertAlign val="baseline"/>
         <sz val="9"/>
         <color theme="1"/>
-        <name val="Calibri"/>
+        <name val="Tinos"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
@@ -5361,8 +5388,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="tblSean" pivot="0" count="2" xr9:uid="{8A27988E-247C-4FF5-8CF3-24D483E6BCB9}">
-      <tableStyleElement type="wholeTable" dxfId="166"/>
-      <tableStyleElement type="headerRow" dxfId="165"/>
+      <tableStyleElement type="wholeTable" dxfId="167"/>
+      <tableStyleElement type="headerRow" dxfId="166"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -5496,239 +5523,240 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{501E7DB2-B92E-4CC2-BCEB-EE8172EEC7CD}" name="Table2" displayName="Table2" ref="A1:X100" totalsRowShown="0" headerRowDxfId="164" dataDxfId="163">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{501E7DB2-B92E-4CC2-BCEB-EE8172EEC7CD}" name="Table2" displayName="Table2" ref="A1:X100" totalsRowShown="0" headerRowDxfId="165" dataDxfId="164">
   <autoFilter ref="A1:X100" xr:uid="{7226A85A-B84E-44B6-A2B9-35F8B3D1B0AD}"/>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{8BB7C1B1-A387-42DD-B62A-6463F9B4DB1E}" name="section" dataDxfId="162"/>
-    <tableColumn id="10" xr3:uid="{0AB8D640-B4D2-494B-BED2-4A3E14C74F51}" name="current" dataDxfId="161"/>
-    <tableColumn id="2" xr3:uid="{B7BBBE47-D702-4B12-B4D0-B4DC9C89DA80}" name="designation" dataDxfId="160"/>
-    <tableColumn id="4" xr3:uid="{72633761-E38D-4E78-B66A-EB488EEC45FE}" name="mass" dataDxfId="159"/>
-    <tableColumn id="5" xr3:uid="{81383B6A-1D00-4389-B077-3692B7443AF5}" name="section_shape" dataDxfId="158"/>
-    <tableColumn id="6" xr3:uid="{E0054499-7630-455F-9B6B-4B3841561793}" name="fabrication_type" dataDxfId="157"/>
-    <tableColumn id="7" xr3:uid="{5E6C6A7D-7730-4A13-A491-CC6C0ADA29B2}" name="d" dataDxfId="156"/>
-    <tableColumn id="8" xr3:uid="{703DEA4F-912E-4B5C-A41D-5C5F3DD2C419}" name="b_f" dataDxfId="155"/>
-    <tableColumn id="11" xr3:uid="{49015D3A-ADDE-42B3-93FD-7BECFEF4721D}" name="t_f" dataDxfId="154"/>
-    <tableColumn id="12" xr3:uid="{73A64AE0-9A1F-4CEF-B227-2AC20B18A872}" name="t_w" dataDxfId="153"/>
-    <tableColumn id="14" xr3:uid="{A0B5F4F6-1155-4C7D-84F3-068454A0AD18}" name="r_1" dataDxfId="152"/>
-    <tableColumn id="3" xr3:uid="{16875B13-7192-48B7-B116-7DC3213820AF}" name="w_1" dataDxfId="151"/>
-    <tableColumn id="9" xr3:uid="{2F8D7D82-72F0-4B8D-88C4-D5DCB4B134E6}" name="r1_or_w1" dataDxfId="150">
+    <tableColumn id="1" xr3:uid="{8BB7C1B1-A387-42DD-B62A-6463F9B4DB1E}" name="section" dataDxfId="163"/>
+    <tableColumn id="10" xr3:uid="{0AB8D640-B4D2-494B-BED2-4A3E14C74F51}" name="current" dataDxfId="162"/>
+    <tableColumn id="2" xr3:uid="{B7BBBE47-D702-4B12-B4D0-B4DC9C89DA80}" name="designation" dataDxfId="161"/>
+    <tableColumn id="4" xr3:uid="{72633761-E38D-4E78-B66A-EB488EEC45FE}" name="mass" dataDxfId="160"/>
+    <tableColumn id="5" xr3:uid="{81383B6A-1D00-4389-B077-3692B7443AF5}" name="section_shape" dataDxfId="159"/>
+    <tableColumn id="6" xr3:uid="{E0054499-7630-455F-9B6B-4B3841561793}" name="fabrication_type" dataDxfId="158"/>
+    <tableColumn id="7" xr3:uid="{5E6C6A7D-7730-4A13-A491-CC6C0ADA29B2}" name="d" dataDxfId="157"/>
+    <tableColumn id="8" xr3:uid="{703DEA4F-912E-4B5C-A41D-5C5F3DD2C419}" name="b_f" dataDxfId="156"/>
+    <tableColumn id="11" xr3:uid="{49015D3A-ADDE-42B3-93FD-7BECFEF4721D}" name="t_f" dataDxfId="155"/>
+    <tableColumn id="12" xr3:uid="{73A64AE0-9A1F-4CEF-B227-2AC20B18A872}" name="t_w" dataDxfId="154"/>
+    <tableColumn id="14" xr3:uid="{A0B5F4F6-1155-4C7D-84F3-068454A0AD18}" name="r_1" dataDxfId="153"/>
+    <tableColumn id="3" xr3:uid="{16875B13-7192-48B7-B116-7DC3213820AF}" name="w_1" dataDxfId="152"/>
+    <tableColumn id="9" xr3:uid="{2F8D7D82-72F0-4B8D-88C4-D5DCB4B134E6}" name="r1_or_w1" dataDxfId="151">
       <calculatedColumnFormula>IF(Table2[[#This Row],[w_1]]="",Table2[[#This Row],[r_1]],Table2[[#This Row],[w_1]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{CDE64B04-1087-4006-8ABA-5519A0A2E1A6}" name="a_g" dataDxfId="149"/>
-    <tableColumn id="24" xr3:uid="{2D05E1A5-4DF5-4B77-B712-A32520E03594}" name="i_x" dataDxfId="148"/>
-    <tableColumn id="25" xr3:uid="{ADCC9581-77CD-425F-9713-77CF780E974C}" name="z_x" dataDxfId="147"/>
-    <tableColumn id="31" xr3:uid="{19238578-BF3D-40CD-BCB0-67E1C5910A34}" name="s_x" dataDxfId="146"/>
-    <tableColumn id="32" xr3:uid="{0CC94EC9-FC32-4F91-85DE-3C0AFF11C283}" name="r_x" dataDxfId="145"/>
-    <tableColumn id="33" xr3:uid="{C4FB763F-BCA9-47F6-A34F-7EDDA9076DFD}" name="i_y" dataDxfId="144"/>
-    <tableColumn id="34" xr3:uid="{9155B815-B357-487F-BEB7-996FEE690B4A}" name="z_y" dataDxfId="143"/>
-    <tableColumn id="41" xr3:uid="{D9852269-7E12-44B1-B8BF-E6669095172C}" name="s_y" dataDxfId="142"/>
-    <tableColumn id="42" xr3:uid="{F9BD9431-13AB-4E83-B633-79B956248CD6}" name="r_y" dataDxfId="141"/>
-    <tableColumn id="43" xr3:uid="{BFBE3126-4FFC-4461-B8DB-C1536E05D0EB}" name="j" dataDxfId="140"/>
-    <tableColumn id="44" xr3:uid="{1A21B9AA-41FF-4280-B2E3-9979A235278E}" name="i_w" dataDxfId="139"/>
+    <tableColumn id="23" xr3:uid="{CDE64B04-1087-4006-8ABA-5519A0A2E1A6}" name="a_g" dataDxfId="150"/>
+    <tableColumn id="24" xr3:uid="{2D05E1A5-4DF5-4B77-B712-A32520E03594}" name="i_x" dataDxfId="149"/>
+    <tableColumn id="25" xr3:uid="{ADCC9581-77CD-425F-9713-77CF780E974C}" name="z_x" dataDxfId="148"/>
+    <tableColumn id="31" xr3:uid="{19238578-BF3D-40CD-BCB0-67E1C5910A34}" name="s_x" dataDxfId="147"/>
+    <tableColumn id="32" xr3:uid="{0CC94EC9-FC32-4F91-85DE-3C0AFF11C283}" name="r_x" dataDxfId="146"/>
+    <tableColumn id="33" xr3:uid="{C4FB763F-BCA9-47F6-A34F-7EDDA9076DFD}" name="i_y" dataDxfId="145"/>
+    <tableColumn id="34" xr3:uid="{9155B815-B357-487F-BEB7-996FEE690B4A}" name="z_y" dataDxfId="144"/>
+    <tableColumn id="41" xr3:uid="{D9852269-7E12-44B1-B8BF-E6669095172C}" name="s_y" dataDxfId="143"/>
+    <tableColumn id="42" xr3:uid="{F9BD9431-13AB-4E83-B633-79B956248CD6}" name="r_y" dataDxfId="142"/>
+    <tableColumn id="43" xr3:uid="{BFBE3126-4FFC-4461-B8DB-C1536E05D0EB}" name="j" dataDxfId="141"/>
+    <tableColumn id="44" xr3:uid="{1A21B9AA-41FF-4280-B2E3-9979A235278E}" name="i_w" dataDxfId="140"/>
   </tableColumns>
   <tableStyleInfo name="tblSean" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{24FCF7EE-CAD4-44DD-8AC7-C47F6D2B600B}" name="Table22" displayName="Table22" ref="A1:W11" totalsRowShown="0" headerRowDxfId="138" dataDxfId="137">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{24FCF7EE-CAD4-44DD-8AC7-C47F6D2B600B}" name="Table22" displayName="Table22" ref="A1:W11" totalsRowShown="0" headerRowDxfId="139" dataDxfId="138">
   <autoFilter ref="A1:W11" xr:uid="{7226A85A-B84E-44B6-A2B9-35F8B3D1B0AD}"/>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{B50E4CB8-E006-43D4-8E9D-5E49D26901F9}" name="section" dataDxfId="136"/>
-    <tableColumn id="3" xr3:uid="{577B01FF-BA84-46CF-9B65-FD306272FCB3}" name="current" dataDxfId="135"/>
-    <tableColumn id="2" xr3:uid="{895E4215-8E1C-4A6E-B9CC-7EB82D5FCD35}" name="designation" dataDxfId="134"/>
-    <tableColumn id="4" xr3:uid="{459ADF1A-6198-41FC-A3BA-021FFCBB1214}" name="mass" dataDxfId="133"/>
-    <tableColumn id="5" xr3:uid="{579A1F98-3A5C-4D6A-B911-9FE3CE85CA99}" name="section_shape" dataDxfId="132"/>
-    <tableColumn id="6" xr3:uid="{F496BD7F-F265-42F2-85B3-6F3807EFC1B0}" name="fabrication_type" dataDxfId="131"/>
-    <tableColumn id="7" xr3:uid="{8C76CE3F-D07A-4571-AC22-E5A4CBDED027}" name="d" dataDxfId="130"/>
-    <tableColumn id="8" xr3:uid="{C5248591-0A4D-4B61-A38E-DE067CC8A7CC}" name="b_f" dataDxfId="129"/>
-    <tableColumn id="11" xr3:uid="{8FAE5072-F594-4D3D-A7A0-7E6EFB7B9345}" name="t_f" dataDxfId="128"/>
-    <tableColumn id="12" xr3:uid="{DE0C7152-58E7-4757-B370-81424ADAE881}" name="t_w" dataDxfId="127"/>
-    <tableColumn id="14" xr3:uid="{2A52F2BF-4E04-4A3A-AAA9-57BCFF0423FA}" name="r_1" dataDxfId="126"/>
-    <tableColumn id="23" xr3:uid="{CB7051BC-ECA8-45AE-8DA8-AE624047A991}" name="a_g" dataDxfId="125"/>
-    <tableColumn id="24" xr3:uid="{CD0D9974-7FDA-444F-BC1E-2BD92935EA8E}" name="i_x" dataDxfId="124"/>
-    <tableColumn id="25" xr3:uid="{32929EA3-CEA4-429F-AABF-5F892A9AAC75}" name="z_x" dataDxfId="123"/>
-    <tableColumn id="31" xr3:uid="{F4445F44-9A63-4ADB-8283-7D0FAB60053E}" name="s_x" dataDxfId="122"/>
-    <tableColumn id="32" xr3:uid="{BB1A59E5-2341-42FA-88EC-1A5DD3F03ABD}" name="r_x" dataDxfId="121"/>
-    <tableColumn id="33" xr3:uid="{50690392-9654-4D08-A275-F42A2AE2C858}" name="i_y" dataDxfId="120"/>
-    <tableColumn id="35" xr3:uid="{4AD32397-8C88-42FD-8630-CBD4405DEC14}" name="z_yl" dataDxfId="119"/>
-    <tableColumn id="36" xr3:uid="{9E868C49-8257-4C05-B452-C3B84674B76D}" name="z_yr" dataDxfId="118"/>
-    <tableColumn id="41" xr3:uid="{BC0E4570-9F58-488E-A156-139EF19BC7CF}" name="s_y" dataDxfId="117"/>
-    <tableColumn id="42" xr3:uid="{A7632747-CC03-469B-B386-EEFD091F3F10}" name="r_y" dataDxfId="116"/>
-    <tableColumn id="43" xr3:uid="{FF0DF439-CC49-40AF-B3A4-F9F76FF75C0A}" name="j" dataDxfId="115"/>
-    <tableColumn id="44" xr3:uid="{908B2CAD-26EB-4AE4-9882-FE33D49A94D0}" name="i_w" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{B50E4CB8-E006-43D4-8E9D-5E49D26901F9}" name="section" dataDxfId="137"/>
+    <tableColumn id="3" xr3:uid="{577B01FF-BA84-46CF-9B65-FD306272FCB3}" name="current" dataDxfId="136"/>
+    <tableColumn id="2" xr3:uid="{895E4215-8E1C-4A6E-B9CC-7EB82D5FCD35}" name="designation" dataDxfId="135"/>
+    <tableColumn id="4" xr3:uid="{459ADF1A-6198-41FC-A3BA-021FFCBB1214}" name="mass" dataDxfId="134"/>
+    <tableColumn id="5" xr3:uid="{579A1F98-3A5C-4D6A-B911-9FE3CE85CA99}" name="section_shape" dataDxfId="133"/>
+    <tableColumn id="6" xr3:uid="{F496BD7F-F265-42F2-85B3-6F3807EFC1B0}" name="fabrication_type" dataDxfId="132"/>
+    <tableColumn id="7" xr3:uid="{8C76CE3F-D07A-4571-AC22-E5A4CBDED027}" name="d" dataDxfId="131"/>
+    <tableColumn id="8" xr3:uid="{C5248591-0A4D-4B61-A38E-DE067CC8A7CC}" name="b_f" dataDxfId="130"/>
+    <tableColumn id="11" xr3:uid="{8FAE5072-F594-4D3D-A7A0-7E6EFB7B9345}" name="t_f" dataDxfId="129"/>
+    <tableColumn id="12" xr3:uid="{DE0C7152-58E7-4757-B370-81424ADAE881}" name="t_w" dataDxfId="128"/>
+    <tableColumn id="14" xr3:uid="{2A52F2BF-4E04-4A3A-AAA9-57BCFF0423FA}" name="r_1" dataDxfId="127"/>
+    <tableColumn id="23" xr3:uid="{CB7051BC-ECA8-45AE-8DA8-AE624047A991}" name="a_g" dataDxfId="126"/>
+    <tableColumn id="24" xr3:uid="{CD0D9974-7FDA-444F-BC1E-2BD92935EA8E}" name="i_x" dataDxfId="125"/>
+    <tableColumn id="25" xr3:uid="{32929EA3-CEA4-429F-AABF-5F892A9AAC75}" name="z_x" dataDxfId="124"/>
+    <tableColumn id="31" xr3:uid="{F4445F44-9A63-4ADB-8283-7D0FAB60053E}" name="s_x" dataDxfId="123"/>
+    <tableColumn id="32" xr3:uid="{BB1A59E5-2341-42FA-88EC-1A5DD3F03ABD}" name="r_x" dataDxfId="122"/>
+    <tableColumn id="33" xr3:uid="{50690392-9654-4D08-A275-F42A2AE2C858}" name="i_y" dataDxfId="121"/>
+    <tableColumn id="35" xr3:uid="{4AD32397-8C88-42FD-8630-CBD4405DEC14}" name="z_yl" dataDxfId="120"/>
+    <tableColumn id="36" xr3:uid="{9E868C49-8257-4C05-B452-C3B84674B76D}" name="z_yr" dataDxfId="119"/>
+    <tableColumn id="41" xr3:uid="{BC0E4570-9F58-488E-A156-139EF19BC7CF}" name="s_y" dataDxfId="118"/>
+    <tableColumn id="42" xr3:uid="{A7632747-CC03-469B-B386-EEFD091F3F10}" name="r_y" dataDxfId="117"/>
+    <tableColumn id="43" xr3:uid="{FF0DF439-CC49-40AF-B3A4-F9F76FF75C0A}" name="j" dataDxfId="116"/>
+    <tableColumn id="44" xr3:uid="{908B2CAD-26EB-4AE4-9882-FE33D49A94D0}" name="i_w" dataDxfId="115"/>
   </tableColumns>
   <tableStyleInfo name="tblSean" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{FF45E8D3-7736-40A7-99D3-559A453C579A}" name="Table12" displayName="Table12" ref="A1:AU66" totalsRowShown="0" headerRowDxfId="113" dataDxfId="112">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{FF45E8D3-7736-40A7-99D3-559A453C579A}" name="Table12" displayName="Table12" ref="A1:AU66" totalsRowShown="0" headerRowDxfId="114" dataDxfId="113">
   <autoFilter ref="A1:AU66" xr:uid="{FF45E8D3-7736-40A7-99D3-559A453C579A}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AU66">
     <sortCondition ref="E1:E66"/>
   </sortState>
   <tableColumns count="47">
-    <tableColumn id="1" xr3:uid="{0E98BFEB-C2F6-42CB-BF8F-C98E1C2E0635}" name="section" dataDxfId="111"/>
-    <tableColumn id="2" xr3:uid="{F8D7BC1B-0DBB-4D99-A300-0E4A90580804}" name="current" dataDxfId="110"/>
-    <tableColumn id="3" xr3:uid="{737CBCED-510B-4F43-B438-2A185FDD6050}" name="designation" dataDxfId="109"/>
-    <tableColumn id="4" xr3:uid="{B458591C-C4BC-4B79-957E-957A01651592}" name="mass" dataDxfId="108"/>
-    <tableColumn id="5" xr3:uid="{1795098C-FBE6-4A95-BF2C-C1D46892588F}" name="section_shape" dataDxfId="107"/>
-    <tableColumn id="6" xr3:uid="{A5CADDBA-1B4B-4115-9488-87017E29615A}" name="fabrication_type" dataDxfId="106"/>
-    <tableColumn id="7" xr3:uid="{238018DD-1F33-4BFE-A2AF-9CECCB06C3F0}" name="b_1" dataDxfId="105"/>
-    <tableColumn id="8" xr3:uid="{9D65AF38-BBE8-40A0-8C16-DFFFAF6CE138}" name="b_2" dataDxfId="104"/>
-    <tableColumn id="9" xr3:uid="{C2203BF0-6699-4823-92F5-390D9CF47F55}" name="t" dataDxfId="103"/>
-    <tableColumn id="10" xr3:uid="{FA82C60C-E6CB-4F75-8515-D3578B68A869}" name="r_1" dataDxfId="102"/>
-    <tableColumn id="11" xr3:uid="{98A4E8DE-21C5-4253-BB88-17B4789DF415}" name="r_2" dataDxfId="101"/>
-    <tableColumn id="14" xr3:uid="{89C8E045-1AD0-433A-B56D-64CF79A5DB3B}" name="a_g" dataDxfId="100"/>
-    <tableColumn id="15" xr3:uid="{0D147C1F-E2B1-4610-8F7F-2F2EDE479941}" name="n_l" dataDxfId="99"/>
-    <tableColumn id="16" xr3:uid="{7837E9B6-E904-4A0F-9F43-CD9FAA135778}" name="n_r" dataDxfId="98"/>
-    <tableColumn id="17" xr3:uid="{F2DB37C1-C66D-4D2D-A8C4-CCCC0ABE5FD7}" name="p_b" dataDxfId="97"/>
-    <tableColumn id="18" xr3:uid="{C3A966E4-6303-4391-9FEA-B96F8F3AB726}" name="p_t" dataDxfId="96"/>
-    <tableColumn id="19" xr3:uid="{06E33A70-92D2-4F18-AECA-57AB30FEB440}" name="i_x" dataDxfId="95"/>
-    <tableColumn id="20" xr3:uid="{9AA65A25-E661-4FAA-AF1D-3D44249D01BF}" name="y_1" dataDxfId="94"/>
-    <tableColumn id="21" xr3:uid="{9A701A27-0B2D-4F45-81BA-39175FEAF0B6}" name="z_x1" dataDxfId="93"/>
-    <tableColumn id="22" xr3:uid="{393FFFA1-B351-4FB1-9277-D50B0910FC0F}" name="y_4" dataDxfId="92"/>
-    <tableColumn id="23" xr3:uid="{2DACC83C-2104-45C1-B9FE-49A63E6E85E4}" name="z_x4" dataDxfId="91"/>
-    <tableColumn id="24" xr3:uid="{5D3F7ABB-7C07-476D-8F2A-742862304A6F}" name="y_5" dataDxfId="90"/>
-    <tableColumn id="25" xr3:uid="{A99B6213-CC3A-4218-A472-E5962B98B458}" name="z_x5" dataDxfId="89"/>
-    <tableColumn id="26" xr3:uid="{75554A80-CD5A-41AC-B6C7-07931FBCB5CB}" name="s_x" dataDxfId="88"/>
-    <tableColumn id="27" xr3:uid="{1C7FD4BF-A120-42D4-9F49-D421ACED02E5}" name="r_x" dataDxfId="87"/>
-    <tableColumn id="28" xr3:uid="{C0B7DB03-B03F-402C-B521-F68B9E6DCB6B}" name="i_y" dataDxfId="86"/>
-    <tableColumn id="29" xr3:uid="{E115797B-BC29-4A13-A6FE-C3C97DFB7135}" name="x_5" dataDxfId="85"/>
-    <tableColumn id="30" xr3:uid="{9E6BF5E6-1873-4844-80B3-E26FC413F5F2}" name="z_y5" dataDxfId="84"/>
-    <tableColumn id="31" xr3:uid="{C645FD7B-D220-4837-8F91-44B3ECD3B912}" name="x_3" dataDxfId="83"/>
-    <tableColumn id="32" xr3:uid="{778B9CFC-50E3-42F0-BF16-6835B2AA19C1}" name="z_y3" dataDxfId="82"/>
-    <tableColumn id="33" xr3:uid="{EE964793-FB8A-4B7C-8D5C-91F411165876}" name="x_2" dataDxfId="81"/>
-    <tableColumn id="34" xr3:uid="{3FE64EFF-34A4-413C-BB0F-062966F896E8}" name="z_y2" dataDxfId="80"/>
-    <tableColumn id="35" xr3:uid="{51D846ED-D7C5-4402-99F2-0DB0F2C24DD3}" name="s_y" dataDxfId="79"/>
-    <tableColumn id="36" xr3:uid="{E2B67361-9A2E-4480-B277-5C2ECFFB818C}" name="r_y" dataDxfId="78"/>
-    <tableColumn id="37" xr3:uid="{F2242E23-7412-4D7B-ACEB-6A0702AD99FA}" name="j" dataDxfId="77"/>
-    <tableColumn id="38" xr3:uid="{1FDDA5D1-FC4C-4923-B73E-C3BC38E38DB6}" name="tan_alpha" dataDxfId="76"/>
-    <tableColumn id="40" xr3:uid="{28747A12-AFEB-4090-B870-6FD912461659}" name="i_n" dataDxfId="75"/>
-    <tableColumn id="41" xr3:uid="{ED8FF4DA-2F9F-4152-8C5A-8E0D76DCA0E5}" name="z_nb" dataDxfId="74"/>
-    <tableColumn id="42" xr3:uid="{3DAA48FF-3532-4FE6-9832-4F6220A62A72}" name="z_nt" dataDxfId="73"/>
-    <tableColumn id="43" xr3:uid="{833FEA35-FCDE-463A-9087-A72AF4E331D5}" name="s_n" dataDxfId="72"/>
-    <tableColumn id="44" xr3:uid="{76B26717-A708-41FD-B8BD-EDA04EF167FC}" name="r_n" dataDxfId="71"/>
-    <tableColumn id="45" xr3:uid="{0B580395-0F1E-4B42-B46E-986CC167FEB3}" name="i_p" dataDxfId="70"/>
-    <tableColumn id="46" xr3:uid="{B9B6BEC6-FD25-41F9-892E-85B8845293E8}" name="z_pl" dataDxfId="69"/>
-    <tableColumn id="47" xr3:uid="{BE8BC5FB-D341-475B-942A-9E50AAA5F9C0}" name="z_pr" dataDxfId="68"/>
-    <tableColumn id="48" xr3:uid="{5BC5C573-CC69-4C9D-9ADE-BA3B1527D7A6}" name="s_p" dataDxfId="67"/>
-    <tableColumn id="49" xr3:uid="{9463694C-A3D5-479B-9FFE-37EE8D4FB591}" name="r_p" dataDxfId="66"/>
-    <tableColumn id="50" xr3:uid="{95621574-0C57-4E53-9BC0-FC033C0A02B9}" name="i_np" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{0E98BFEB-C2F6-42CB-BF8F-C98E1C2E0635}" name="section" dataDxfId="112"/>
+    <tableColumn id="2" xr3:uid="{F8D7BC1B-0DBB-4D99-A300-0E4A90580804}" name="current" dataDxfId="111"/>
+    <tableColumn id="3" xr3:uid="{737CBCED-510B-4F43-B438-2A185FDD6050}" name="designation" dataDxfId="110"/>
+    <tableColumn id="4" xr3:uid="{B458591C-C4BC-4B79-957E-957A01651592}" name="mass" dataDxfId="109"/>
+    <tableColumn id="5" xr3:uid="{1795098C-FBE6-4A95-BF2C-C1D46892588F}" name="section_shape" dataDxfId="108"/>
+    <tableColumn id="6" xr3:uid="{A5CADDBA-1B4B-4115-9488-87017E29615A}" name="fabrication_type" dataDxfId="107"/>
+    <tableColumn id="7" xr3:uid="{238018DD-1F33-4BFE-A2AF-9CECCB06C3F0}" name="b_1" dataDxfId="106"/>
+    <tableColumn id="8" xr3:uid="{9D65AF38-BBE8-40A0-8C16-DFFFAF6CE138}" name="b_2" dataDxfId="105"/>
+    <tableColumn id="9" xr3:uid="{C2203BF0-6699-4823-92F5-390D9CF47F55}" name="t" dataDxfId="104"/>
+    <tableColumn id="10" xr3:uid="{FA82C60C-E6CB-4F75-8515-D3578B68A869}" name="r_1" dataDxfId="103"/>
+    <tableColumn id="11" xr3:uid="{98A4E8DE-21C5-4253-BB88-17B4789DF415}" name="r_2" dataDxfId="102"/>
+    <tableColumn id="14" xr3:uid="{89C8E045-1AD0-433A-B56D-64CF79A5DB3B}" name="a_g" dataDxfId="101"/>
+    <tableColumn id="15" xr3:uid="{0D147C1F-E2B1-4610-8F7F-2F2EDE479941}" name="n_l" dataDxfId="100"/>
+    <tableColumn id="16" xr3:uid="{7837E9B6-E904-4A0F-9F43-CD9FAA135778}" name="n_r" dataDxfId="99"/>
+    <tableColumn id="17" xr3:uid="{F2DB37C1-C66D-4D2D-A8C4-CCCC0ABE5FD7}" name="p_b" dataDxfId="98"/>
+    <tableColumn id="18" xr3:uid="{C3A966E4-6303-4391-9FEA-B96F8F3AB726}" name="p_t" dataDxfId="97"/>
+    <tableColumn id="19" xr3:uid="{06E33A70-92D2-4F18-AECA-57AB30FEB440}" name="i_x" dataDxfId="96"/>
+    <tableColumn id="20" xr3:uid="{9AA65A25-E661-4FAA-AF1D-3D44249D01BF}" name="y_1" dataDxfId="95"/>
+    <tableColumn id="21" xr3:uid="{9A701A27-0B2D-4F45-81BA-39175FEAF0B6}" name="z_x1" dataDxfId="94"/>
+    <tableColumn id="22" xr3:uid="{393FFFA1-B351-4FB1-9277-D50B0910FC0F}" name="y_4" dataDxfId="93"/>
+    <tableColumn id="23" xr3:uid="{2DACC83C-2104-45C1-B9FE-49A63E6E85E4}" name="z_x4" dataDxfId="92"/>
+    <tableColumn id="24" xr3:uid="{5D3F7ABB-7C07-476D-8F2A-742862304A6F}" name="y_5" dataDxfId="91"/>
+    <tableColumn id="25" xr3:uid="{A99B6213-CC3A-4218-A472-E5962B98B458}" name="z_x5" dataDxfId="90"/>
+    <tableColumn id="26" xr3:uid="{75554A80-CD5A-41AC-B6C7-07931FBCB5CB}" name="s_x" dataDxfId="89"/>
+    <tableColumn id="27" xr3:uid="{1C7FD4BF-A120-42D4-9F49-D421ACED02E5}" name="r_x" dataDxfId="88"/>
+    <tableColumn id="28" xr3:uid="{C0B7DB03-B03F-402C-B521-F68B9E6DCB6B}" name="i_y" dataDxfId="87"/>
+    <tableColumn id="29" xr3:uid="{E115797B-BC29-4A13-A6FE-C3C97DFB7135}" name="x_5" dataDxfId="86"/>
+    <tableColumn id="30" xr3:uid="{9E6BF5E6-1873-4844-80B3-E26FC413F5F2}" name="z_y5" dataDxfId="85"/>
+    <tableColumn id="31" xr3:uid="{C645FD7B-D220-4837-8F91-44B3ECD3B912}" name="x_3" dataDxfId="84"/>
+    <tableColumn id="32" xr3:uid="{778B9CFC-50E3-42F0-BF16-6835B2AA19C1}" name="z_y3" dataDxfId="83"/>
+    <tableColumn id="33" xr3:uid="{EE964793-FB8A-4B7C-8D5C-91F411165876}" name="x_2" dataDxfId="82"/>
+    <tableColumn id="34" xr3:uid="{3FE64EFF-34A4-413C-BB0F-062966F896E8}" name="z_y2" dataDxfId="81"/>
+    <tableColumn id="35" xr3:uid="{51D846ED-D7C5-4402-99F2-0DB0F2C24DD3}" name="s_y" dataDxfId="80"/>
+    <tableColumn id="36" xr3:uid="{E2B67361-9A2E-4480-B277-5C2ECFFB818C}" name="r_y" dataDxfId="79"/>
+    <tableColumn id="37" xr3:uid="{F2242E23-7412-4D7B-ACEB-6A0702AD99FA}" name="j" dataDxfId="78"/>
+    <tableColumn id="38" xr3:uid="{1FDDA5D1-FC4C-4923-B73E-C3BC38E38DB6}" name="tan_alpha" dataDxfId="77"/>
+    <tableColumn id="40" xr3:uid="{28747A12-AFEB-4090-B870-6FD912461659}" name="i_n" dataDxfId="76"/>
+    <tableColumn id="41" xr3:uid="{ED8FF4DA-2F9F-4152-8C5A-8E0D76DCA0E5}" name="z_nb" dataDxfId="75"/>
+    <tableColumn id="42" xr3:uid="{3DAA48FF-3532-4FE6-9832-4F6220A62A72}" name="z_nt" dataDxfId="74"/>
+    <tableColumn id="43" xr3:uid="{833FEA35-FCDE-463A-9087-A72AF4E331D5}" name="s_n" dataDxfId="73"/>
+    <tableColumn id="44" xr3:uid="{76B26717-A708-41FD-B8BD-EDA04EF167FC}" name="r_n" dataDxfId="72"/>
+    <tableColumn id="45" xr3:uid="{0B580395-0F1E-4B42-B46E-986CC167FEB3}" name="i_p" dataDxfId="71"/>
+    <tableColumn id="46" xr3:uid="{B9B6BEC6-FD25-41F9-892E-85B8845293E8}" name="z_pl" dataDxfId="70"/>
+    <tableColumn id="47" xr3:uid="{BE8BC5FB-D341-475B-942A-9E50AAA5F9C0}" name="z_pr" dataDxfId="69"/>
+    <tableColumn id="48" xr3:uid="{5BC5C573-CC69-4C9D-9ADE-BA3B1527D7A6}" name="s_p" dataDxfId="68"/>
+    <tableColumn id="49" xr3:uid="{9463694C-A3D5-479B-9FFE-37EE8D4FB591}" name="r_p" dataDxfId="67"/>
+    <tableColumn id="50" xr3:uid="{95621574-0C57-4E53-9BC0-FC033C0A02B9}" name="i_np" dataDxfId="66"/>
   </tableColumns>
   <tableStyleInfo name="tblSean" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F856F8D5-18F2-4A4D-B287-05A7E0FF4BE1}" name="Table6" displayName="Table6" ref="A1:W214" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F856F8D5-18F2-4A4D-B287-05A7E0FF4BE1}" name="Table6" displayName="Table6" ref="A1:W214" totalsRowShown="0" headerRowDxfId="65" dataDxfId="64">
   <autoFilter ref="A1:W214" xr:uid="{F856F8D5-18F2-4A4D-B287-05A7E0FF4BE1}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U5">
     <sortCondition ref="C1:C5"/>
   </sortState>
   <tableColumns count="23">
-    <tableColumn id="1" xr3:uid="{E2925810-9C25-4132-BD5C-0C5A42D6A5EC}" name="section" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{29DF28F2-F045-4FB5-9C6A-137EF8CD95BE}" name="current" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{E0220977-C835-4F23-84EE-414C1FB0AAE1}" name="designation" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{4AD71210-471B-4703-AB9B-F486971BA2A1}" name="mass" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{DD9D9038-D97E-4758-8DD0-B14CA71C812F}" name="section_shape" dataDxfId="58"/>
-    <tableColumn id="6" xr3:uid="{02672C8D-03B0-4D8B-8619-4432D5969A4A}" name="fabrication_type" dataDxfId="57"/>
-    <tableColumn id="9" xr3:uid="{4A188572-EC44-4443-9EC8-90B6ED8DA804}" name="grade" dataDxfId="56"/>
-    <tableColumn id="8" xr3:uid="{827373FC-F25E-4349-AD07-EAFEB6B115C2}" name="standard" dataDxfId="55"/>
-    <tableColumn id="11" xr3:uid="{3A7583DF-88D0-45A3-97CD-7706449B782E}" name="d" dataDxfId="54"/>
-    <tableColumn id="12" xr3:uid="{4AD1418E-6E9D-439F-8B4F-3B3CFA20B544}" name="b" dataDxfId="53"/>
-    <tableColumn id="13" xr3:uid="{287D0ED0-248B-4DD9-9BCD-A6EE331603B8}" name="t" dataDxfId="52"/>
-    <tableColumn id="7" xr3:uid="{1CC4C8E3-54B6-464C-A529-82FE3496DB64}" name="r_ext" dataDxfId="51"/>
-    <tableColumn id="16" xr3:uid="{77049593-28F1-4D83-8C14-F10F3E66A5D7}" name="a_g" dataDxfId="50"/>
-    <tableColumn id="17" xr3:uid="{3240AB16-E873-4A2B-B3DA-861D829AE31F}" name="i_x" dataDxfId="49"/>
-    <tableColumn id="18" xr3:uid="{8B09D638-0194-4AC0-BBD4-61DD2A62D3AB}" name="z_x" dataDxfId="48"/>
-    <tableColumn id="19" xr3:uid="{8E60B5AE-75F6-43E6-8862-AE98480D9A53}" name="s_x" dataDxfId="47"/>
-    <tableColumn id="20" xr3:uid="{14931501-0531-428B-B2FA-9C5C9B8D963D}" name="r_x" dataDxfId="46"/>
-    <tableColumn id="21" xr3:uid="{C394B290-F7E3-4AA0-AFC7-C2D2C979FDD1}" name="i_y" dataDxfId="45"/>
-    <tableColumn id="22" xr3:uid="{4E103565-1C69-4681-81A6-991D62E282C9}" name="z_y" dataDxfId="44"/>
-    <tableColumn id="23" xr3:uid="{B4451F83-E157-42F5-81A7-D27C6265A445}" name="s_y" dataDxfId="43"/>
-    <tableColumn id="24" xr3:uid="{C7B5BFBB-6023-44E8-9480-8F7249B60E9C}" name="r_y" dataDxfId="42"/>
-    <tableColumn id="27" xr3:uid="{121A9941-351F-4C3C-A65A-73C4C311794F}" name="j" dataDxfId="41"/>
-    <tableColumn id="28" xr3:uid="{88B2FE0E-4A60-40F1-8D6E-111D544F2617}" name="c" dataDxfId="40"/>
+    <tableColumn id="1" xr3:uid="{E2925810-9C25-4132-BD5C-0C5A42D6A5EC}" name="section" dataDxfId="63"/>
+    <tableColumn id="2" xr3:uid="{29DF28F2-F045-4FB5-9C6A-137EF8CD95BE}" name="current" dataDxfId="62"/>
+    <tableColumn id="3" xr3:uid="{E0220977-C835-4F23-84EE-414C1FB0AAE1}" name="designation" dataDxfId="61"/>
+    <tableColumn id="4" xr3:uid="{4AD71210-471B-4703-AB9B-F486971BA2A1}" name="mass" dataDxfId="60"/>
+    <tableColumn id="5" xr3:uid="{DD9D9038-D97E-4758-8DD0-B14CA71C812F}" name="section_shape" dataDxfId="59"/>
+    <tableColumn id="6" xr3:uid="{02672C8D-03B0-4D8B-8619-4432D5969A4A}" name="fabrication_type" dataDxfId="58"/>
+    <tableColumn id="9" xr3:uid="{4A188572-EC44-4443-9EC8-90B6ED8DA804}" name="grade" dataDxfId="57"/>
+    <tableColumn id="8" xr3:uid="{827373FC-F25E-4349-AD07-EAFEB6B115C2}" name="standard" dataDxfId="56"/>
+    <tableColumn id="11" xr3:uid="{3A7583DF-88D0-45A3-97CD-7706449B782E}" name="d" dataDxfId="55"/>
+    <tableColumn id="12" xr3:uid="{4AD1418E-6E9D-439F-8B4F-3B3CFA20B544}" name="b" dataDxfId="54"/>
+    <tableColumn id="13" xr3:uid="{287D0ED0-248B-4DD9-9BCD-A6EE331603B8}" name="t" dataDxfId="53"/>
+    <tableColumn id="7" xr3:uid="{1CC4C8E3-54B6-464C-A529-82FE3496DB64}" name="r_ext" dataDxfId="52"/>
+    <tableColumn id="16" xr3:uid="{77049593-28F1-4D83-8C14-F10F3E66A5D7}" name="a_g" dataDxfId="51"/>
+    <tableColumn id="17" xr3:uid="{3240AB16-E873-4A2B-B3DA-861D829AE31F}" name="i_x" dataDxfId="50"/>
+    <tableColumn id="18" xr3:uid="{8B09D638-0194-4AC0-BBD4-61DD2A62D3AB}" name="z_x" dataDxfId="49"/>
+    <tableColumn id="19" xr3:uid="{8E60B5AE-75F6-43E6-8862-AE98480D9A53}" name="s_x" dataDxfId="48"/>
+    <tableColumn id="20" xr3:uid="{14931501-0531-428B-B2FA-9C5C9B8D963D}" name="r_x" dataDxfId="47"/>
+    <tableColumn id="21" xr3:uid="{C394B290-F7E3-4AA0-AFC7-C2D2C979FDD1}" name="i_y" dataDxfId="46"/>
+    <tableColumn id="22" xr3:uid="{4E103565-1C69-4681-81A6-991D62E282C9}" name="z_y" dataDxfId="45"/>
+    <tableColumn id="23" xr3:uid="{B4451F83-E157-42F5-81A7-D27C6265A445}" name="s_y" dataDxfId="44"/>
+    <tableColumn id="24" xr3:uid="{C7B5BFBB-6023-44E8-9480-8F7249B60E9C}" name="r_y" dataDxfId="43"/>
+    <tableColumn id="27" xr3:uid="{121A9941-351F-4C3C-A65A-73C4C311794F}" name="j" dataDxfId="42"/>
+    <tableColumn id="28" xr3:uid="{88B2FE0E-4A60-40F1-8D6E-111D544F2617}" name="c" dataDxfId="41"/>
   </tableColumns>
   <tableStyleInfo name="tblSean" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{82015ECB-7CED-4ACD-A99C-225C1D660049}" name="Table9" displayName="Table9" ref="A1:Q74" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{82015ECB-7CED-4ACD-A99C-225C1D660049}" name="Table9" displayName="Table9" ref="A1:Q74" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
   <autoFilter ref="A1:Q74" xr:uid="{82015ECB-7CED-4ACD-A99C-225C1D660049}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q74">
     <sortCondition ref="G1:G74"/>
   </sortState>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{F989E24A-2895-403A-95D8-FB6D57B33393}" name="section" dataDxfId="37"/>
-    <tableColumn id="2" xr3:uid="{3A3AA581-72B7-4C71-92ED-58FF0AF8C58F}" name="current" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{4AF474D4-D6CD-478F-9C12-9E3BD9498538}" name="designation" dataDxfId="35"/>
-    <tableColumn id="4" xr3:uid="{FB925A7C-C5BD-4C4F-B3B7-409904034742}" name="mass" dataDxfId="34"/>
-    <tableColumn id="5" xr3:uid="{671391B3-7819-4686-B553-6816137ABD4C}" name="section_shape" dataDxfId="33"/>
-    <tableColumn id="6" xr3:uid="{D1A5F5F4-1AC1-4423-A8A6-FFF97CAE9132}" name="fabrication_type" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{370D76B4-ED4B-4369-B0DA-F466EE63D50C}" name="grade" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{7D379C42-B6F9-4886-BC19-6BB4717591C7}" name="standard" dataDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{F287B4A8-95A8-4F80-AA3C-6CB66011704D}" name="d" dataDxfId="29"/>
-    <tableColumn id="10" xr3:uid="{9B5E365E-AF5E-4F63-8A33-962C2AB3671D}" name="t" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{85DE6BC4-7DB1-431E-9156-2965CE49DB00}" name="a_g" dataDxfId="27"/>
-    <tableColumn id="13" xr3:uid="{D2661048-444D-4C95-9F11-0677EC8A1982}" name="i" dataDxfId="26"/>
-    <tableColumn id="14" xr3:uid="{F0DAF1A3-96B3-492E-AFF5-13A74AD474B2}" name="z" dataDxfId="25"/>
-    <tableColumn id="15" xr3:uid="{905A8923-FED3-4886-87C3-EFFB3C0C84D5}" name="s" dataDxfId="24"/>
-    <tableColumn id="16" xr3:uid="{89747857-0C0B-4369-A11D-5A861AD3C77F}" name="r" dataDxfId="23"/>
-    <tableColumn id="17" xr3:uid="{6720023D-EA79-4ECC-BBC2-79CB176A6FA2}" name="j" dataDxfId="22"/>
-    <tableColumn id="18" xr3:uid="{792A3F36-2BD7-4DC0-9411-D3763E15297D}" name="c" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{F989E24A-2895-403A-95D8-FB6D57B33393}" name="section" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{3A3AA581-72B7-4C71-92ED-58FF0AF8C58F}" name="current" dataDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{4AF474D4-D6CD-478F-9C12-9E3BD9498538}" name="designation" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{FB925A7C-C5BD-4C4F-B3B7-409904034742}" name="mass" dataDxfId="35"/>
+    <tableColumn id="5" xr3:uid="{671391B3-7819-4686-B553-6816137ABD4C}" name="section_shape" dataDxfId="34"/>
+    <tableColumn id="6" xr3:uid="{D1A5F5F4-1AC1-4423-A8A6-FFF97CAE9132}" name="fabrication_type" dataDxfId="33"/>
+    <tableColumn id="7" xr3:uid="{370D76B4-ED4B-4369-B0DA-F466EE63D50C}" name="grade" dataDxfId="32"/>
+    <tableColumn id="8" xr3:uid="{7D379C42-B6F9-4886-BC19-6BB4717591C7}" name="standard" dataDxfId="31"/>
+    <tableColumn id="9" xr3:uid="{F287B4A8-95A8-4F80-AA3C-6CB66011704D}" name="d" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{9B5E365E-AF5E-4F63-8A33-962C2AB3671D}" name="t" dataDxfId="29"/>
+    <tableColumn id="12" xr3:uid="{85DE6BC4-7DB1-431E-9156-2965CE49DB00}" name="a_g" dataDxfId="28"/>
+    <tableColumn id="13" xr3:uid="{D2661048-444D-4C95-9F11-0677EC8A1982}" name="i" dataDxfId="27"/>
+    <tableColumn id="14" xr3:uid="{F0DAF1A3-96B3-492E-AFF5-13A74AD474B2}" name="z" dataDxfId="26"/>
+    <tableColumn id="15" xr3:uid="{905A8923-FED3-4886-87C3-EFFB3C0C84D5}" name="s" dataDxfId="25"/>
+    <tableColumn id="16" xr3:uid="{89747857-0C0B-4369-A11D-5A861AD3C77F}" name="r" dataDxfId="24"/>
+    <tableColumn id="17" xr3:uid="{6720023D-EA79-4ECC-BBC2-79CB176A6FA2}" name="j" dataDxfId="23"/>
+    <tableColumn id="18" xr3:uid="{792A3F36-2BD7-4DC0-9411-D3763E15297D}" name="c" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="tblSean" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0B154D11-09EB-4C87-921D-9FAEB2520622}" name="Table3" displayName="Table3" ref="A1:G63" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0B154D11-09EB-4C87-921D-9FAEB2520622}" name="Table3" displayName="Table3" ref="A1:G63" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
   <autoFilter ref="A1:G63" xr:uid="{0B154D11-09EB-4C87-921D-9FAEB2520622}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F624C6BE-779F-496C-A6A5-C90E3B909046}" name="standard" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{F4DBA019-F123-4B98-A615-C1C293EAF7F6}" name="current" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{49F22BD6-5E2F-4DCD-B8F2-753E49B729CD}" name="form" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{D21D031E-2102-48DD-8FDF-9B85CD1F2DC4}" name="grade" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{287A8683-8D3D-499F-9ADF-C78622D53763}" name="t" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{77FEE7B2-5CF2-4D12-B956-927382100BB2}" name="f_y" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{8A7B2AE8-B6A6-43AC-8500-1C07B6953654}" name="f_u" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{F624C6BE-779F-496C-A6A5-C90E3B909046}" name="standard" dataDxfId="19"/>
+    <tableColumn id="7" xr3:uid="{F4DBA019-F123-4B98-A615-C1C293EAF7F6}" name="current" dataDxfId="18"/>
+    <tableColumn id="6" xr3:uid="{49F22BD6-5E2F-4DCD-B8F2-753E49B729CD}" name="form" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{D21D031E-2102-48DD-8FDF-9B85CD1F2DC4}" name="grade" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{287A8683-8D3D-499F-9ADF-C78622D53763}" name="t" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{77FEE7B2-5CF2-4D12-B956-927382100BB2}" name="f_y" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{8A7B2AE8-B6A6-43AC-8500-1C07B6953654}" name="f_u" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="tblSean" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{33323D96-8D05-4556-B6B1-AFCB559AD4C2}" name="Table4" displayName="Table4" ref="A1:A21" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{33323D96-8D05-4556-B6B1-AFCB559AD4C2}" name="Table4" displayName="Table4" ref="A1:A21" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A1:A21" xr:uid="{33323D96-8D05-4556-B6B1-AFCB559AD4C2}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{30D98F40-E00D-49DD-B117-7321D335A518}" name="thickness" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{30D98F40-E00D-49DD-B117-7321D335A518}" name="thickness" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="tblSean" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D70FA64A-2C15-4122-9CB7-517E837789DD}" name="Table5" displayName="Table5" ref="A1:A11" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D70FA64A-2C15-4122-9CB7-517E837789DD}" name="Table5" displayName="Table5" ref="A1:A11" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="A1:A11" xr:uid="{D70FA64A-2C15-4122-9CB7-517E837789DD}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3CB5E7CA-7DA9-4A14-81EC-A5B9BB9E0DFB}" name="leg_size" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{3CB5E7CA-7DA9-4A14-81EC-A5B9BB9E0DFB}" name="leg_size" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="tblSean" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{43A45A43-E759-48F9-AA1A-CB9E7279BA23}" name="Table7" displayName="Table7" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D9" xr:uid="{43A45A43-E759-48F9-AA1A-CB9E7279BA23}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{2EE18AA7-3C68-4DF5-9A13-87B6A633C1FE}" name="grade" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{A0CA93C9-68D9-4869-9DAD-4C97DB84FFA7}" name="d_f" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{A00732D1-A557-4E3F-BFCC-691336453C69}" name="f_yf" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{9EEECFE1-D0E2-4C53-B695-0EA0E87596AC}" name="f_uf" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{43A45A43-E759-48F9-AA1A-CB9E7279BA23}" name="Table7" displayName="Table7" ref="A1:E9" totalsRowShown="0" headerRowDxfId="2" dataDxfId="6">
+  <autoFilter ref="A1:E9" xr:uid="{43A45A43-E759-48F9-AA1A-CB9E7279BA23}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{2EE18AA7-3C68-4DF5-9A13-87B6A633C1FE}" name="grade" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{A0CA93C9-68D9-4869-9DAD-4C97DB84FFA7}" name="d_f" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{A00732D1-A557-4E3F-BFCC-691336453C69}" name="f_yf" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{9EEECFE1-D0E2-4C53-B695-0EA0E87596AC}" name="f_uf" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{95BC92BA-2E09-430D-B6D1-4825A5031A59}" name="k_rd" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="tblSean" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5775,110 +5803,16 @@
         <a:srgbClr val="70342E"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="sean_fonts">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Roboto"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Tinos"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office 2013 - 2022">
@@ -6039,20 +5973,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="12" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="7" max="12" width="7.42578125" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="17" width="12.7109375" customWidth="1"/>
+    <col min="18" max="18" width="7.42578125" customWidth="1"/>
+    <col min="19" max="21" width="12.7109375" customWidth="1"/>
+    <col min="22" max="22" width="7.42578125" customWidth="1"/>
+    <col min="23" max="24" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
@@ -13458,22 +13392,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="11" width="6.7109375" customWidth="1"/>
+    <col min="12" max="12" width="9.5703125" customWidth="1"/>
+    <col min="13" max="15" width="11.28515625" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" customWidth="1"/>
+    <col min="17" max="17" width="9.5703125" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" customWidth="1"/>
+    <col min="20" max="20" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" customWidth="1"/>
+    <col min="22" max="23" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -14276,36 +14209,36 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="40" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="42" max="45" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="11" width="6.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
+    <col min="13" max="16" width="6.7109375" customWidth="1"/>
+    <col min="17" max="17" width="11.28515625" customWidth="1"/>
+    <col min="18" max="18" width="6.7109375" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="6.7109375" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" customWidth="1"/>
+    <col min="22" max="23" width="6.7109375" customWidth="1"/>
+    <col min="24" max="24" width="11.28515625" customWidth="1"/>
+    <col min="25" max="25" width="6.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.28515625" customWidth="1"/>
+    <col min="27" max="27" width="6.7109375" customWidth="1"/>
+    <col min="28" max="28" width="11.28515625" customWidth="1"/>
+    <col min="29" max="29" width="6.7109375" customWidth="1"/>
+    <col min="30" max="30" width="11.28515625" customWidth="1"/>
+    <col min="31" max="31" width="6.7109375" customWidth="1"/>
+    <col min="32" max="33" width="11.28515625" customWidth="1"/>
+    <col min="34" max="34" width="6.7109375" customWidth="1"/>
+    <col min="35" max="40" width="11.28515625" customWidth="1"/>
+    <col min="41" max="41" width="6.7109375" customWidth="1"/>
+    <col min="42" max="45" width="11.28515625" customWidth="1"/>
+    <col min="46" max="46" width="6.7109375" customWidth="1"/>
+    <col min="47" max="47" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:47" x14ac:dyDescent="0.25">
@@ -23765,20 +23698,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="16.140625" customWidth="1"/>
-    <col min="9" max="11" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.7109375" customWidth="1"/>
-    <col min="13" max="16" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="20" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" customWidth="1"/>
+    <col min="6" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="12" width="6.7109375" customWidth="1"/>
+    <col min="13" max="16" width="11.28515625" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" customWidth="1"/>
+    <col min="18" max="20" width="11.28515625" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" customWidth="1"/>
+    <col min="22" max="23" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.25">
@@ -38993,18 +38924,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="14" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="10" width="6.7109375" customWidth="1"/>
+    <col min="11" max="14" width="11.28515625" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" customWidth="1"/>
+    <col min="16" max="17" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -42947,13 +42878,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -44423,7 +44354,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -44549,7 +44480,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -44617,34 +44548,38 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF28B45-6FA5-47FF-9023-4500F42C558D}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="40" t="s">
         <v>530</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="40" t="s">
         <v>525</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="40" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="40" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="38" t="s">
         <v>527</v>
       </c>
@@ -44657,8 +44592,11 @@
       <c r="D2" s="37">
         <v>800000000</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="38" t="s">
         <v>527</v>
       </c>
@@ -44671,8 +44609,11 @@
       <c r="D3" s="37">
         <v>800000000</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="38" t="s">
         <v>527</v>
       </c>
@@ -44685,8 +44626,11 @@
       <c r="D4" s="37">
         <v>830000000</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="38" t="s">
         <v>527</v>
       </c>
@@ -44699,8 +44643,11 @@
       <c r="D5" s="37">
         <v>830000000</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="38" t="s">
         <v>528</v>
       </c>
@@ -44713,8 +44660,11 @@
       <c r="D6" s="37">
         <v>400000000</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="38" t="s">
         <v>528</v>
       </c>
@@ -44727,8 +44677,11 @@
       <c r="D7" s="37">
         <v>400000000</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="38" t="s">
         <v>529</v>
       </c>
@@ -44741,8 +44694,11 @@
       <c r="D8" s="37">
         <v>1040000000</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="34">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="38" t="s">
         <v>529</v>
       </c>
@@ -44754,6 +44710,9 @@
       </c>
       <c r="D9" s="37">
         <v>1040000000</v>
+      </c>
+      <c r="E9" s="34">
+        <v>0.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data for steel grades to Pa (SI units).
Update tests as well to suit.
</commit_message>
<xml_diff>
--- a/src/utilityscripts/steel/data/steel_data.xlsx
+++ b/src/utilityscripts/steel/data/steel_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sean.kane\programming\utilityscripts\src\utilityscripts\steel\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF815038-825E-45D7-8810-9D70A27C3F0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE10BF53-CF20-4937-8DA6-4743826E5AEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="135" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{2C3896B0-8573-48C6-A232-BE22E9D89C30}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{2C3896B0-8573-48C6-A232-BE22E9D89C30}"/>
   </bookViews>
   <sheets>
     <sheet name="is" sheetId="1" r:id="rId1"/>
@@ -1661,9 +1661,9 @@
     <numFmt numFmtId="168" formatCode="##0.00E+00&quot; m⁴&quot;"/>
     <numFmt numFmtId="169" formatCode="##0.00E+00&quot; m³&quot;"/>
     <numFmt numFmtId="170" formatCode="##0.00E+00&quot; m⁶&quot;"/>
-    <numFmt numFmtId="171" formatCode="0.0"/>
     <numFmt numFmtId="172" formatCode="0.000"/>
     <numFmt numFmtId="173" formatCode="0&quot; kg / m&quot;"/>
+    <numFmt numFmtId="175" formatCode="0.00E+0&quot; Pa&quot;"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -1825,9 +1825,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1843,13 +1840,36 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="168">
     <dxf>
+      <numFmt numFmtId="175" formatCode="0.00E+0&quot; Pa&quot;"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="175" formatCode="0.00E+0&quot; Pa&quot;"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1867,18 +1887,6 @@
         <name val="Roboto"/>
         <scheme val="major"/>
       </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1901,14 +1909,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode="0.0"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -5721,42 +5721,42 @@
     <tableColumn id="6" xr3:uid="{49F22BD6-5E2F-4DCD-B8F2-753E49B729CD}" name="form" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{D21D031E-2102-48DD-8FDF-9B85CD1F2DC4}" name="grade" dataDxfId="16"/>
     <tableColumn id="3" xr3:uid="{287A8683-8D3D-499F-9ADF-C78622D53763}" name="t" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{77FEE7B2-5CF2-4D12-B956-927382100BB2}" name="f_y" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{8A7B2AE8-B6A6-43AC-8500-1C07B6953654}" name="f_u" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{77FEE7B2-5CF2-4D12-B956-927382100BB2}" name="f_y" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{8A7B2AE8-B6A6-43AC-8500-1C07B6953654}" name="f_u" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="tblSean" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{33323D96-8D05-4556-B6B1-AFCB559AD4C2}" name="Table4" displayName="Table4" ref="A1:A21" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{33323D96-8D05-4556-B6B1-AFCB559AD4C2}" name="Table4" displayName="Table4" ref="A1:A21" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="A1:A21" xr:uid="{33323D96-8D05-4556-B6B1-AFCB559AD4C2}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{30D98F40-E00D-49DD-B117-7321D335A518}" name="thickness" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{30D98F40-E00D-49DD-B117-7321D335A518}" name="thickness" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="tblSean" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D70FA64A-2C15-4122-9CB7-517E837789DD}" name="Table5" displayName="Table5" ref="A1:A11" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{D70FA64A-2C15-4122-9CB7-517E837789DD}" name="Table5" displayName="Table5" ref="A1:A11" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:A11" xr:uid="{D70FA64A-2C15-4122-9CB7-517E837789DD}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{3CB5E7CA-7DA9-4A14-81EC-A5B9BB9E0DFB}" name="leg_size" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{3CB5E7CA-7DA9-4A14-81EC-A5B9BB9E0DFB}" name="leg_size" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="tblSean" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{43A45A43-E759-48F9-AA1A-CB9E7279BA23}" name="Table7" displayName="Table7" ref="A1:E9" totalsRowShown="0" headerRowDxfId="2" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{43A45A43-E759-48F9-AA1A-CB9E7279BA23}" name="Table7" displayName="Table7" ref="A1:E9" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:E9" xr:uid="{43A45A43-E759-48F9-AA1A-CB9E7279BA23}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{2EE18AA7-3C68-4DF5-9A13-87B6A633C1FE}" name="grade" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{A0CA93C9-68D9-4869-9DAD-4C97DB84FFA7}" name="d_f" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{A00732D1-A557-4E3F-BFCC-691336453C69}" name="f_yf" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{9EEECFE1-D0E2-4C53-B695-0EA0E87596AC}" name="f_uf" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{95BC92BA-2E09-430D-B6D1-4825A5031A59}" name="k_rd" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{2EE18AA7-3C68-4DF5-9A13-87B6A633C1FE}" name="grade" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{A0CA93C9-68D9-4869-9DAD-4C97DB84FFA7}" name="d_f" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{A00732D1-A557-4E3F-BFCC-691336453C69}" name="f_yf" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{9EEECFE1-D0E2-4C53-B695-0EA0E87596AC}" name="f_uf" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{95BC92BA-2E09-430D-B6D1-4825A5031A59}" name="k_rd" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="tblSean" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -42872,8 +42872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4418AB-7087-489E-B717-DDAB43816858}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42883,8 +42883,7 @@
     <col min="3" max="3" width="15.7109375" customWidth="1"/>
     <col min="4" max="4" width="10.140625" customWidth="1"/>
     <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="6" max="7" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -42926,11 +42925,11 @@
       <c r="E2" s="34">
         <v>0</v>
       </c>
-      <c r="F2" s="35">
-        <v>250</v>
-      </c>
-      <c r="G2" s="35">
-        <v>320</v>
+      <c r="F2" s="40">
+        <v>250000000</v>
+      </c>
+      <c r="G2" s="40">
+        <v>320000000</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -42949,11 +42948,11 @@
       <c r="E3" s="34">
         <v>0.1</v>
       </c>
-      <c r="F3" s="35">
-        <v>250</v>
-      </c>
-      <c r="G3" s="35">
-        <v>320</v>
+      <c r="F3" s="40">
+        <v>250000000</v>
+      </c>
+      <c r="G3" s="40">
+        <v>320000000</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -42972,11 +42971,11 @@
       <c r="E4" s="34">
         <v>0</v>
       </c>
-      <c r="F4" s="35">
-        <v>350</v>
-      </c>
-      <c r="G4" s="35">
-        <v>430</v>
+      <c r="F4" s="40">
+        <v>350000000</v>
+      </c>
+      <c r="G4" s="40">
+        <v>430000000</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -42995,11 +42994,11 @@
       <c r="E5" s="34">
         <v>0.1</v>
       </c>
-      <c r="F5" s="35">
-        <v>350</v>
-      </c>
-      <c r="G5" s="35">
-        <v>430</v>
+      <c r="F5" s="40">
+        <v>350000000</v>
+      </c>
+      <c r="G5" s="40">
+        <v>430000000</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -43018,11 +43017,11 @@
       <c r="E6" s="34">
         <v>0</v>
       </c>
-      <c r="F6" s="35">
-        <v>450</v>
-      </c>
-      <c r="G6" s="35">
-        <v>500</v>
+      <c r="F6" s="40">
+        <v>450000000</v>
+      </c>
+      <c r="G6" s="40">
+        <v>500000000</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -43041,11 +43040,11 @@
       <c r="E7" s="34">
         <v>0.1</v>
       </c>
-      <c r="F7" s="35">
-        <v>450</v>
-      </c>
-      <c r="G7" s="35">
-        <v>500</v>
+      <c r="F7" s="40">
+        <v>450000000</v>
+      </c>
+      <c r="G7" s="40">
+        <v>500000000</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -43064,11 +43063,11 @@
       <c r="E8" s="34">
         <v>0</v>
       </c>
-      <c r="F8" s="35">
-        <v>280</v>
-      </c>
-      <c r="G8" s="35">
-        <v>410</v>
+      <c r="F8" s="40">
+        <v>280000000</v>
+      </c>
+      <c r="G8" s="40">
+        <v>410000000</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -43087,11 +43086,11 @@
       <c r="E9" s="34">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F9" s="35">
-        <v>280</v>
-      </c>
-      <c r="G9" s="35">
-        <v>410</v>
+      <c r="F9" s="40">
+        <v>280000000</v>
+      </c>
+      <c r="G9" s="40">
+        <v>410000000</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -43110,11 +43109,11 @@
       <c r="E10" s="34">
         <v>8.0099999999999998E-3</v>
       </c>
-      <c r="F10" s="35">
-        <v>260</v>
-      </c>
-      <c r="G10" s="35">
-        <v>410</v>
+      <c r="F10" s="40">
+        <v>260000000</v>
+      </c>
+      <c r="G10" s="40">
+        <v>410000000</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -43133,11 +43132,11 @@
       <c r="E11" s="34">
         <v>1.2E-2</v>
       </c>
-      <c r="F11" s="35">
-        <v>260</v>
-      </c>
-      <c r="G11" s="35">
-        <v>410</v>
+      <c r="F11" s="40">
+        <v>260000000</v>
+      </c>
+      <c r="G11" s="40">
+        <v>410000000</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -43156,11 +43155,11 @@
       <c r="E12" s="34">
         <v>1.201E-2</v>
       </c>
-      <c r="F12" s="35">
-        <v>250</v>
-      </c>
-      <c r="G12" s="35">
-        <v>410</v>
+      <c r="F12" s="40">
+        <v>250000000</v>
+      </c>
+      <c r="G12" s="40">
+        <v>410000000</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -43179,11 +43178,11 @@
       <c r="E13" s="34">
         <v>0.05</v>
       </c>
-      <c r="F13" s="35">
-        <v>250</v>
-      </c>
-      <c r="G13" s="35">
-        <v>410</v>
+      <c r="F13" s="40">
+        <v>250000000</v>
+      </c>
+      <c r="G13" s="40">
+        <v>410000000</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -43202,11 +43201,11 @@
       <c r="E14" s="34">
         <v>5.0009999999999999E-2</v>
       </c>
-      <c r="F14" s="35">
-        <v>240</v>
-      </c>
-      <c r="G14" s="35">
-        <v>410</v>
+      <c r="F14" s="40">
+        <v>240000000</v>
+      </c>
+      <c r="G14" s="40">
+        <v>410000000</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -43225,11 +43224,11 @@
       <c r="E15" s="34">
         <v>0.08</v>
       </c>
-      <c r="F15" s="35">
-        <v>240</v>
-      </c>
-      <c r="G15" s="35">
-        <v>410</v>
+      <c r="F15" s="40">
+        <v>240000000</v>
+      </c>
+      <c r="G15" s="40">
+        <v>410000000</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -43248,11 +43247,11 @@
       <c r="E16" s="34">
         <v>8.0010000000000012E-2</v>
       </c>
-      <c r="F16" s="35">
-        <v>230</v>
-      </c>
-      <c r="G16" s="35">
-        <v>410</v>
+      <c r="F16" s="40">
+        <v>230000000</v>
+      </c>
+      <c r="G16" s="40">
+        <v>410000000</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -43271,11 +43270,11 @@
       <c r="E17" s="34">
         <v>0.15</v>
       </c>
-      <c r="F17" s="35">
-        <v>230</v>
-      </c>
-      <c r="G17" s="35">
-        <v>410</v>
+      <c r="F17" s="40">
+        <v>230000000</v>
+      </c>
+      <c r="G17" s="40">
+        <v>410000000</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -43294,11 +43293,11 @@
       <c r="E18" s="34">
         <v>0</v>
       </c>
-      <c r="F18" s="35">
-        <v>200</v>
-      </c>
-      <c r="G18" s="35">
-        <v>300</v>
+      <c r="F18" s="40">
+        <v>200000000</v>
+      </c>
+      <c r="G18" s="40">
+        <v>300000000</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -43317,11 +43316,11 @@
       <c r="E19" s="34">
         <v>1.2E-2</v>
       </c>
-      <c r="F19" s="35">
-        <v>200</v>
-      </c>
-      <c r="G19" s="35">
-        <v>300</v>
+      <c r="F19" s="40">
+        <v>200000000</v>
+      </c>
+      <c r="G19" s="40">
+        <v>300000000</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -43340,11 +43339,11 @@
       <c r="E20" s="34">
         <v>0</v>
       </c>
-      <c r="F20" s="35">
-        <v>320</v>
-      </c>
-      <c r="G20" s="35">
-        <v>430</v>
+      <c r="F20" s="40">
+        <v>320000000</v>
+      </c>
+      <c r="G20" s="40">
+        <v>430000000</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -43363,11 +43362,11 @@
       <c r="E21" s="34">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F21" s="35">
-        <v>320</v>
-      </c>
-      <c r="G21" s="35">
-        <v>430</v>
+      <c r="F21" s="40">
+        <v>320000000</v>
+      </c>
+      <c r="G21" s="40">
+        <v>430000000</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -43386,11 +43385,11 @@
       <c r="E22" s="34">
         <v>8.0099999999999998E-3</v>
       </c>
-      <c r="F22" s="35">
-        <v>310</v>
-      </c>
-      <c r="G22" s="35">
-        <v>430</v>
+      <c r="F22" s="40">
+        <v>310000000</v>
+      </c>
+      <c r="G22" s="40">
+        <v>430000000</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -43409,11 +43408,11 @@
       <c r="E23" s="34">
         <v>1.2E-2</v>
       </c>
-      <c r="F23" s="35">
-        <v>310</v>
-      </c>
-      <c r="G23" s="35">
-        <v>430</v>
+      <c r="F23" s="40">
+        <v>310000000</v>
+      </c>
+      <c r="G23" s="40">
+        <v>430000000</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -43432,11 +43431,11 @@
       <c r="E24" s="34">
         <v>1.201E-2</v>
       </c>
-      <c r="F24" s="35">
-        <v>300</v>
-      </c>
-      <c r="G24" s="35">
-        <v>430</v>
+      <c r="F24" s="40">
+        <v>300000000</v>
+      </c>
+      <c r="G24" s="40">
+        <v>430000000</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -43455,11 +43454,11 @@
       <c r="E25" s="34">
         <v>0.02</v>
       </c>
-      <c r="F25" s="35">
-        <v>300</v>
-      </c>
-      <c r="G25" s="35">
-        <v>430</v>
+      <c r="F25" s="40">
+        <v>300000000</v>
+      </c>
+      <c r="G25" s="40">
+        <v>430000000</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -43478,11 +43477,11 @@
       <c r="E26" s="34">
         <v>2.001E-2</v>
       </c>
-      <c r="F26" s="35">
-        <v>280</v>
-      </c>
-      <c r="G26" s="35">
-        <v>430</v>
+      <c r="F26" s="40">
+        <v>280000000</v>
+      </c>
+      <c r="G26" s="40">
+        <v>430000000</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -43501,11 +43500,11 @@
       <c r="E27" s="34">
         <v>0.05</v>
       </c>
-      <c r="F27" s="35">
-        <v>280</v>
-      </c>
-      <c r="G27" s="35">
-        <v>430</v>
+      <c r="F27" s="40">
+        <v>280000000</v>
+      </c>
+      <c r="G27" s="40">
+        <v>430000000</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -43524,11 +43523,11 @@
       <c r="E28" s="34">
         <v>5.0009999999999999E-2</v>
       </c>
-      <c r="F28" s="35">
-        <v>270</v>
-      </c>
-      <c r="G28" s="35">
-        <v>430</v>
+      <c r="F28" s="40">
+        <v>270000000</v>
+      </c>
+      <c r="G28" s="40">
+        <v>430000000</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -43547,11 +43546,11 @@
       <c r="E29" s="34">
         <v>0.08</v>
       </c>
-      <c r="F29" s="35">
-        <v>270</v>
-      </c>
-      <c r="G29" s="35">
-        <v>430</v>
+      <c r="F29" s="40">
+        <v>270000000</v>
+      </c>
+      <c r="G29" s="40">
+        <v>430000000</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -43570,11 +43569,11 @@
       <c r="E30" s="34">
         <v>8.0010000000000012E-2</v>
       </c>
-      <c r="F30" s="35">
-        <v>260</v>
-      </c>
-      <c r="G30" s="35">
-        <v>430</v>
+      <c r="F30" s="40">
+        <v>260000000</v>
+      </c>
+      <c r="G30" s="40">
+        <v>430000000</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -43593,11 +43592,11 @@
       <c r="E31" s="34">
         <v>0.15</v>
       </c>
-      <c r="F31" s="35">
-        <v>260</v>
-      </c>
-      <c r="G31" s="35">
-        <v>430</v>
+      <c r="F31" s="40">
+        <v>260000000</v>
+      </c>
+      <c r="G31" s="40">
+        <v>430000000</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -43616,11 +43615,11 @@
       <c r="E32" s="34">
         <v>0</v>
       </c>
-      <c r="F32" s="35">
-        <v>360</v>
-      </c>
-      <c r="G32" s="35">
-        <v>450</v>
+      <c r="F32" s="40">
+        <v>360000000</v>
+      </c>
+      <c r="G32" s="40">
+        <v>450000000</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -43639,11 +43638,11 @@
       <c r="E33" s="34">
         <v>1.2E-2</v>
       </c>
-      <c r="F33" s="35">
-        <v>360</v>
-      </c>
-      <c r="G33" s="35">
-        <v>450</v>
+      <c r="F33" s="40">
+        <v>360000000</v>
+      </c>
+      <c r="G33" s="40">
+        <v>450000000</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -43662,11 +43661,11 @@
       <c r="E34" s="34">
         <v>1.201E-2</v>
       </c>
-      <c r="F34" s="35">
-        <v>350</v>
-      </c>
-      <c r="G34" s="35">
-        <v>450</v>
+      <c r="F34" s="40">
+        <v>350000000</v>
+      </c>
+      <c r="G34" s="40">
+        <v>450000000</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -43685,11 +43684,11 @@
       <c r="E35" s="34">
         <v>0.02</v>
       </c>
-      <c r="F35" s="35">
-        <v>350</v>
-      </c>
-      <c r="G35" s="35">
-        <v>450</v>
+      <c r="F35" s="40">
+        <v>350000000</v>
+      </c>
+      <c r="G35" s="40">
+        <v>450000000</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -43708,11 +43707,11 @@
       <c r="E36" s="34">
         <v>2.001E-2</v>
       </c>
-      <c r="F36" s="35">
-        <v>340</v>
-      </c>
-      <c r="G36" s="35">
-        <v>450</v>
+      <c r="F36" s="40">
+        <v>340000000</v>
+      </c>
+      <c r="G36" s="40">
+        <v>450000000</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -43731,11 +43730,11 @@
       <c r="E37" s="34">
         <v>0.08</v>
       </c>
-      <c r="F37" s="35">
-        <v>340</v>
-      </c>
-      <c r="G37" s="35">
-        <v>450</v>
+      <c r="F37" s="40">
+        <v>340000000</v>
+      </c>
+      <c r="G37" s="40">
+        <v>450000000</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -43754,11 +43753,11 @@
       <c r="E38" s="34">
         <v>8.0010000000000012E-2</v>
       </c>
-      <c r="F38" s="35">
-        <v>330</v>
-      </c>
-      <c r="G38" s="35">
-        <v>450</v>
+      <c r="F38" s="40">
+        <v>330000000</v>
+      </c>
+      <c r="G38" s="40">
+        <v>450000000</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -43777,11 +43776,11 @@
       <c r="E39" s="34">
         <v>0.15</v>
       </c>
-      <c r="F39" s="35">
-        <v>330</v>
-      </c>
-      <c r="G39" s="35">
-        <v>450</v>
+      <c r="F39" s="40">
+        <v>330000000</v>
+      </c>
+      <c r="G39" s="40">
+        <v>450000000</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -43800,11 +43799,11 @@
       <c r="E40" s="34">
         <v>0</v>
       </c>
-      <c r="F40" s="35">
-        <v>400</v>
-      </c>
-      <c r="G40" s="35">
-        <v>480</v>
+      <c r="F40" s="40">
+        <v>400000000</v>
+      </c>
+      <c r="G40" s="40">
+        <v>480000000</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -43823,11 +43822,11 @@
       <c r="E41" s="34">
         <v>1.2E-2</v>
       </c>
-      <c r="F41" s="35">
-        <v>400</v>
-      </c>
-      <c r="G41" s="35">
-        <v>480</v>
+      <c r="F41" s="40">
+        <v>400000000</v>
+      </c>
+      <c r="G41" s="40">
+        <v>480000000</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -43846,11 +43845,11 @@
       <c r="E42" s="34">
         <v>1.201E-2</v>
       </c>
-      <c r="F42" s="35">
-        <v>380</v>
-      </c>
-      <c r="G42" s="35">
-        <v>480</v>
+      <c r="F42" s="40">
+        <v>380000000</v>
+      </c>
+      <c r="G42" s="40">
+        <v>480000000</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -43869,11 +43868,11 @@
       <c r="E43" s="34">
         <v>0.02</v>
       </c>
-      <c r="F43" s="35">
-        <v>380</v>
-      </c>
-      <c r="G43" s="35">
-        <v>480</v>
+      <c r="F43" s="40">
+        <v>380000000</v>
+      </c>
+      <c r="G43" s="40">
+        <v>480000000</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -43892,11 +43891,11 @@
       <c r="E44" s="34">
         <v>2.001E-2</v>
       </c>
-      <c r="F44" s="35">
-        <v>360</v>
-      </c>
-      <c r="G44" s="35">
-        <v>480</v>
+      <c r="F44" s="40">
+        <v>360000000</v>
+      </c>
+      <c r="G44" s="40">
+        <v>480000000</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -43915,11 +43914,11 @@
       <c r="E45" s="34">
         <v>0.08</v>
       </c>
-      <c r="F45" s="35">
-        <v>360</v>
-      </c>
-      <c r="G45" s="35">
-        <v>480</v>
+      <c r="F45" s="40">
+        <v>360000000</v>
+      </c>
+      <c r="G45" s="40">
+        <v>480000000</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -43938,11 +43937,11 @@
       <c r="E46" s="34">
         <v>0</v>
       </c>
-      <c r="F46" s="35">
-        <v>450</v>
-      </c>
-      <c r="G46" s="35">
-        <v>520</v>
+      <c r="F46" s="40">
+        <v>450000000</v>
+      </c>
+      <c r="G46" s="40">
+        <v>520000000</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -43961,11 +43960,11 @@
       <c r="E47" s="34">
         <v>0.02</v>
       </c>
-      <c r="F47" s="35">
-        <v>450</v>
-      </c>
-      <c r="G47" s="35">
-        <v>520</v>
+      <c r="F47" s="40">
+        <v>450000000</v>
+      </c>
+      <c r="G47" s="40">
+        <v>520000000</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -43984,11 +43983,11 @@
       <c r="E48" s="34">
         <v>2.001E-2</v>
       </c>
-      <c r="F48" s="35">
-        <v>420</v>
-      </c>
-      <c r="G48" s="35">
-        <v>500</v>
+      <c r="F48" s="40">
+        <v>420000000</v>
+      </c>
+      <c r="G48" s="40">
+        <v>500000000</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -44007,11 +44006,11 @@
       <c r="E49" s="34">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="F49" s="35">
-        <v>420</v>
-      </c>
-      <c r="G49" s="35">
-        <v>500</v>
+      <c r="F49" s="40">
+        <v>420000000</v>
+      </c>
+      <c r="G49" s="40">
+        <v>500000000</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -44030,11 +44029,11 @@
       <c r="E50" s="34">
         <v>3.2009999999999997E-2</v>
       </c>
-      <c r="F50" s="35">
-        <v>400</v>
-      </c>
-      <c r="G50" s="35">
-        <v>500</v>
+      <c r="F50" s="40">
+        <v>400000000</v>
+      </c>
+      <c r="G50" s="40">
+        <v>500000000</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -44053,11 +44052,11 @@
       <c r="E51" s="34">
         <v>0.05</v>
       </c>
-      <c r="F51" s="35">
-        <v>400</v>
-      </c>
-      <c r="G51" s="35">
-        <v>500</v>
+      <c r="F51" s="40">
+        <v>400000000</v>
+      </c>
+      <c r="G51" s="40">
+        <v>500000000</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -44076,11 +44075,11 @@
       <c r="E52" s="34">
         <v>0</v>
       </c>
-      <c r="F52" s="35">
-        <v>360</v>
-      </c>
-      <c r="G52" s="35">
-        <v>480</v>
+      <c r="F52" s="40">
+        <v>360000000</v>
+      </c>
+      <c r="G52" s="40">
+        <v>480000000</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -44099,11 +44098,11 @@
       <c r="E53" s="34">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="F53" s="35">
-        <v>360</v>
-      </c>
-      <c r="G53" s="35">
-        <v>480</v>
+      <c r="F53" s="40">
+        <v>360000000</v>
+      </c>
+      <c r="G53" s="40">
+        <v>480000000</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -44122,11 +44121,11 @@
       <c r="E54" s="34">
         <v>1.1009999999999999E-2</v>
       </c>
-      <c r="F54" s="35">
-        <v>340</v>
-      </c>
-      <c r="G54" s="35">
-        <v>480</v>
+      <c r="F54" s="40">
+        <v>340000000</v>
+      </c>
+      <c r="G54" s="40">
+        <v>480000000</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -44145,11 +44144,11 @@
       <c r="E55" s="34">
         <v>0.04</v>
       </c>
-      <c r="F55" s="35">
-        <v>340</v>
-      </c>
-      <c r="G55" s="35">
-        <v>480</v>
+      <c r="F55" s="40">
+        <v>340000000</v>
+      </c>
+      <c r="G55" s="40">
+        <v>480000000</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -44168,11 +44167,11 @@
       <c r="E56" s="34">
         <v>4.0009999999999997E-2</v>
       </c>
-      <c r="F56" s="35">
-        <v>330</v>
-      </c>
-      <c r="G56" s="35">
-        <v>480</v>
+      <c r="F56" s="40">
+        <v>330000000</v>
+      </c>
+      <c r="G56" s="40">
+        <v>480000000</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -44191,11 +44190,11 @@
       <c r="E57" s="34">
         <v>0.1</v>
       </c>
-      <c r="F57" s="35">
-        <v>330</v>
-      </c>
-      <c r="G57" s="35">
-        <v>480</v>
+      <c r="F57" s="40">
+        <v>330000000</v>
+      </c>
+      <c r="G57" s="40">
+        <v>480000000</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -44214,11 +44213,11 @@
       <c r="E58" s="34">
         <v>0</v>
       </c>
-      <c r="F58" s="35">
-        <v>320</v>
-      </c>
-      <c r="G58" s="35">
-        <v>440</v>
+      <c r="F58" s="40">
+        <v>320000000</v>
+      </c>
+      <c r="G58" s="40">
+        <v>440000000</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -44237,11 +44236,11 @@
       <c r="E59" s="34">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="F59" s="35">
-        <v>320</v>
-      </c>
-      <c r="G59" s="35">
-        <v>440</v>
+      <c r="F59" s="40">
+        <v>320000000</v>
+      </c>
+      <c r="G59" s="40">
+        <v>440000000</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -44260,11 +44259,11 @@
       <c r="E60" s="34">
         <v>1.1009999999999999E-2</v>
       </c>
-      <c r="F60" s="35">
-        <v>300</v>
-      </c>
-      <c r="G60" s="35">
-        <v>440</v>
+      <c r="F60" s="40">
+        <v>300000000</v>
+      </c>
+      <c r="G60" s="40">
+        <v>440000000</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -44283,11 +44282,11 @@
       <c r="E61" s="34">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="F61" s="35">
-        <v>300</v>
-      </c>
-      <c r="G61" s="35">
-        <v>440</v>
+      <c r="F61" s="40">
+        <v>300000000</v>
+      </c>
+      <c r="G61" s="40">
+        <v>440000000</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -44306,11 +44305,11 @@
       <c r="E62" s="34">
         <v>1.7010000000000001E-2</v>
       </c>
-      <c r="F62" s="35">
-        <v>280</v>
-      </c>
-      <c r="G62" s="35">
-        <v>440</v>
+      <c r="F62" s="40">
+        <v>280000000</v>
+      </c>
+      <c r="G62" s="40">
+        <v>440000000</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -44329,11 +44328,11 @@
       <c r="E63" s="34">
         <v>0.1</v>
       </c>
-      <c r="F63" s="35">
-        <v>280</v>
-      </c>
-      <c r="G63" s="35">
-        <v>440</v>
+      <c r="F63" s="40">
+        <v>280000000</v>
+      </c>
+      <c r="G63" s="40">
+        <v>440000000</v>
       </c>
     </row>
   </sheetData>
@@ -44363,102 +44362,102 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36">
+      <c r="A2" s="35">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36">
+      <c r="A3" s="35">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36">
+      <c r="A4" s="35">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36">
+      <c r="A5" s="35">
         <v>0.01</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36">
+      <c r="A6" s="35">
         <v>1.2E-2</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36">
+      <c r="A7" s="35">
         <v>1.6E-2</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36">
+      <c r="A8" s="35">
         <v>0.02</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36">
+      <c r="A9" s="35">
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="36">
+      <c r="A10" s="35">
         <v>2.8000000000000001E-2</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36">
+      <c r="A11" s="35">
         <v>3.2000000000000001E-2</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="36">
+      <c r="A12" s="35">
         <v>3.5999999999999997E-2</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="36">
+      <c r="A13" s="35">
         <v>0.04</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36">
+      <c r="A14" s="35">
         <v>4.4999999999999998E-2</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="36">
+      <c r="A15" s="35">
         <v>0.05</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="36">
+      <c r="A16" s="35">
         <v>5.5E-2</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36">
+      <c r="A17" s="35">
         <v>0.06</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="36">
+      <c r="A18" s="35">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="36">
+      <c r="A19" s="35">
         <v>0.08</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="36">
+      <c r="A20" s="35">
         <v>0.09</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="36">
+      <c r="A21" s="35">
         <v>0.1</v>
       </c>
     </row>
@@ -44489,52 +44488,52 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36">
+      <c r="A2" s="35">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36">
+      <c r="A3" s="35">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="36">
+      <c r="A4" s="35">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="36">
+      <c r="A5" s="35">
         <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36">
+      <c r="A6" s="35">
         <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="36">
+      <c r="A7" s="35">
         <v>0.01</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="36">
+      <c r="A8" s="35">
         <v>1.2E-2</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="36">
+      <c r="A9" s="35">
         <v>1.6E-2</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="36">
+      <c r="A10" s="35">
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="36">
+      <c r="A11" s="35">
         <v>0.02</v>
       </c>
     </row>
@@ -44550,8 +44549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF28B45-6FA5-47FF-9023-4500F42C558D}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44563,33 +44562,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
         <v>530</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="39" t="s">
         <v>525</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="39" t="s">
         <v>526</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="39" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="37" t="s">
         <v>527</v>
       </c>
-      <c r="B2" s="36">
+      <c r="B2" s="35">
         <v>0</v>
       </c>
-      <c r="C2" s="37">
+      <c r="C2" s="36">
         <v>640000000</v>
       </c>
-      <c r="D2" s="37">
+      <c r="D2" s="36">
         <v>800000000</v>
       </c>
       <c r="E2" s="34">
@@ -44597,16 +44596,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="37" t="s">
         <v>527</v>
       </c>
-      <c r="B3" s="36">
+      <c r="B3" s="35">
         <v>1.5999989999999999E-2</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="36">
         <v>640000000</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="36">
         <v>800000000</v>
       </c>
       <c r="E3" s="34">
@@ -44614,16 +44613,16 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="37" t="s">
         <v>527</v>
       </c>
-      <c r="B4" s="39">
+      <c r="B4" s="38">
         <v>1.6E-2</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="36">
         <v>660000000</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="36">
         <v>830000000</v>
       </c>
       <c r="E4" s="34">
@@ -44631,16 +44630,16 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="37" t="s">
         <v>527</v>
       </c>
-      <c r="B5" s="39">
+      <c r="B5" s="38">
         <v>0.1</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="36">
         <v>660000000</v>
       </c>
-      <c r="D5" s="37">
+      <c r="D5" s="36">
         <v>830000000</v>
       </c>
       <c r="E5" s="34">
@@ -44648,16 +44647,16 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="37" t="s">
         <v>528</v>
       </c>
-      <c r="B6" s="39">
+      <c r="B6" s="38">
         <v>0</v>
       </c>
-      <c r="C6" s="37">
+      <c r="C6" s="36">
         <v>240000000</v>
       </c>
-      <c r="D6" s="37">
+      <c r="D6" s="36">
         <v>400000000</v>
       </c>
       <c r="E6" s="34">
@@ -44665,16 +44664,16 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="37" t="s">
         <v>528</v>
       </c>
-      <c r="B7" s="39">
+      <c r="B7" s="38">
         <v>0.1</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="36">
         <v>240000000</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="36">
         <v>400000000</v>
       </c>
       <c r="E7" s="34">
@@ -44682,16 +44681,16 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="38" t="s">
+      <c r="A8" s="37" t="s">
         <v>529</v>
       </c>
-      <c r="B8" s="39">
+      <c r="B8" s="38">
         <v>0</v>
       </c>
-      <c r="C8" s="37">
+      <c r="C8" s="36">
         <v>940000000</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="36">
         <v>1040000000</v>
       </c>
       <c r="E8" s="34">
@@ -44699,16 +44698,16 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="38" t="s">
+      <c r="A9" s="37" t="s">
         <v>529</v>
       </c>
-      <c r="B9" s="39">
+      <c r="B9" s="38">
         <v>0.1</v>
       </c>
-      <c r="C9" s="37">
+      <c r="C9" s="36">
         <v>940000000</v>
       </c>
-      <c r="D9" s="37">
+      <c r="D9" s="36">
         <v>1040000000</v>
       </c>
       <c r="E9" s="34">

</xml_diff>